<commit_message>
Southland Trial initial build
</commit_message>
<xml_diff>
--- a/Southland Trial/SysSettings.xlsx
+++ b/Southland Trial/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\Southland Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1775968E-3978-469E-B745-57481C56E27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4894A8-C664-436C-98F5-6BE6DD2384E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12855" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="164">
   <si>
     <t>IMP*Z</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>Allows dummy variables if set to 1</t>
+  </si>
+  <si>
+    <t>~TFM_INS-txt</t>
   </si>
 </sst>
 </file>
@@ -16280,7 +16283,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16497,8 +16500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16683,7 +16686,7 @@
   <dimension ref="B3:E10"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16750,7 +16753,7 @@
         <v>57</v>
       </c>
       <c r="C10" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>162</v>
@@ -16768,8 +16771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16793,8 +16796,8 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="str">
-        <f>IF($A$1=1,"~TFM_MIG","~TFM_UPD")</f>
-        <v>~TFM_UPD</v>
+        <f>IF($A$1=1,"~TFM_MIG","~TFM_INS")</f>
+        <v>~TFM_INS</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -17281,7 +17284,7 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -18391,7 +18394,7 @@
   <dimension ref="B1:I14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>